<commit_message>
didn't actually upload updated version
</commit_message>
<xml_diff>
--- a/space usage analysis/space usage analysis.xlsx
+++ b/space usage analysis/space usage analysis.xlsx
@@ -3730,8 +3730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>